<commit_message>
Cleaning up Order list
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{9EC149C7-7858-4882-B5DB-44E1F22FFD21}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{4C88BD53-F838-422B-8A2E-DE3DC63B5DCF}"/>
   <bookViews>
-    <workbookView xWindow="20592" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21528" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -422,9 +422,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="[$EUR]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="[$EUR]\ #,##0.0"/>
-    <numFmt numFmtId="167" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$EUR]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$EUR]\ #,##0.0"/>
+    <numFmt numFmtId="166" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -578,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,7 +601,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -610,31 +610,31 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1342,101 +1342,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="40">
-        <f>'V-Slots and Wheels List'!F18</f>
+      <c r="B5" s="37">
+        <f>'V-Slots and Wheels List'!F17</f>
         <v>172.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="37">
         <f>'Component Part List'!E28</f>
         <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="37">
         <f>'Fasteners List'!E33</f>
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="40"/>
+      <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="36">
         <f>SUM(B5:B8)</f>
         <v>556.5</v>
       </c>
@@ -1447,7 +1447,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="35" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1459,6 +1459,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{3FC4702C-93F0-44D6-B76F-6AAFF00BF8D8}"/>
+    <hyperlink ref="A5" location="'V-Slots and Wheels List'!A1" display="V-Slots and Wheels Standard Price:" xr:uid="{A29DA81D-7B91-4E4B-B65C-26042F66F5C3}"/>
+    <hyperlink ref="A6" location="'Component Part List'!A1" display="Components Example Price:" xr:uid="{9EB7D7DD-AF1E-400D-9685-4CB15F55C14B}"/>
+    <hyperlink ref="A7" location="'Fasteners List'!A1" display="Fastners Estimated Retail Price:" xr:uid="{542B85DB-19D3-4E26-AF3D-CED032A5654A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
@@ -1468,16 +1471,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
-  <dimension ref="A6:F18"/>
+  <dimension ref="A6:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
@@ -1518,16 +1519,16 @@
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="42" t="s">
         <v>96</v>
       </c>
       <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="43">
         <v>80</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="44">
         <f>E8</f>
         <v>80</v>
       </c>
@@ -1539,12 +1540,12 @@
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="42"/>
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -1646,11 +1647,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F17" s="33">
         <f>SUM(F8:F16)</f>
         <v>172.5</v>
       </c>
@@ -1669,7 +1670,8 @@
     <hyperlink ref="C12" r:id="rId5" xr:uid="{9E7C5336-3FF2-4EE3-AFBF-F1C41492D09C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1677,9 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2137,9 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A389EA4-5A5F-4A9C-B048-2EB9BC969CA3}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
added bundle order list
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{4C88BD53-F838-422B-8A2E-DE3DC63B5DCF}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{17BADE8F-41F0-4DDF-B5EF-911DFC44AC30}"/>
   <bookViews>
-    <workbookView xWindow="21528" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22464" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
     <sheet name="V-Slots and Wheels List" sheetId="5" r:id="rId2"/>
     <sheet name="Component Part List" sheetId="3" r:id="rId3"/>
     <sheet name="Fasteners List" sheetId="4" r:id="rId4"/>
+    <sheet name="Bundle Order List" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
   <si>
     <t>Part Name</t>
   </si>
@@ -415,6 +416,129 @@
   </si>
   <si>
     <t>Bulk Price</t>
+  </si>
+  <si>
+    <t>V-King Bundle List - Send this list to info@ratrig.com to order</t>
+  </si>
+  <si>
+    <t>Estamated price for the bundle - 250 EUR - Ask for price confirmation</t>
+  </si>
+  <si>
+    <t>Mailto:</t>
+  </si>
+  <si>
+    <t>info@ratrig.com</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>HW1113BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028 L Bracket </t>
+  </si>
+  <si>
+    <t>HW1303BC</t>
+  </si>
+  <si>
+    <t>28mm X 20mm corner bracket</t>
+  </si>
+  <si>
+    <t>HW1212WK</t>
+  </si>
+  <si>
+    <t>V-Slot Big Wheels - Extreme</t>
+  </si>
+  <si>
+    <t>V-Slot Big Wheels - Standard</t>
+  </si>
+  <si>
+    <t>Mechatronical components</t>
+  </si>
+  <si>
+    <t>HW1078EC</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Timing Belt GT2 6mm</t>
+  </si>
+  <si>
+    <t>HW1037GC</t>
+  </si>
+  <si>
+    <t>Meter Timing belt for XYZ</t>
+  </si>
+  <si>
+    <t>Timing Motor GT2 Pulley 20T</t>
+  </si>
+  <si>
+    <t>HW1035WC</t>
+  </si>
+  <si>
+    <t>Motor Timing Pulleys</t>
+  </si>
+  <si>
+    <t>Fastners and Bearings</t>
+  </si>
+  <si>
+    <t>HW1251NC</t>
+  </si>
+  <si>
+    <t>HW1508NC</t>
+  </si>
+  <si>
+    <t>HW1373NC</t>
+  </si>
+  <si>
+    <t>HW1505SC</t>
+  </si>
+  <si>
+    <t>HW1502SC</t>
+  </si>
+  <si>
+    <t>HW1561NC</t>
+  </si>
+  <si>
+    <t>HW1074NC</t>
+  </si>
+  <si>
+    <t>HW1039NC</t>
+  </si>
+  <si>
+    <t>HW1111NC</t>
+  </si>
+  <si>
+    <t>HW1315NC</t>
+  </si>
+  <si>
+    <t>HW1285SC</t>
+  </si>
+  <si>
+    <t>HW1209WC</t>
+  </si>
+  <si>
+    <t>Ball Bearing - 625 ZZ</t>
+  </si>
+  <si>
+    <t>Bearings</t>
+  </si>
+  <si>
+    <t>Controller components</t>
+  </si>
+  <si>
+    <t>HW1351EC</t>
+  </si>
+  <si>
+    <t>110/220VAC - 24V PSU 240W Min</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Part Number</t>
   </si>
 </sst>
 </file>
@@ -426,7 +550,7 @@
     <numFmt numFmtId="165" formatCode="[$EUR]\ #,##0.0"/>
     <numFmt numFmtId="166" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +617,13 @@
       <name val="Aharoni"/>
       <charset val="177"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -503,19 +634,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,15 +696,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -583,21 +713,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -618,6 +741,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,9 +765,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -661,7 +795,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>15239</xdr:rowOff>
+      <xdr:rowOff>121919</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5154506" cy="2899409"/>
     <xdr:pic>
@@ -691,7 +825,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2575559"/>
+          <a:off x="0" y="2819399"/>
           <a:ext cx="5154506" cy="2899409"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -705,7 +839,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4442460" cy="4442460"/>
@@ -779,6 +913,126 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1516380</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2651760" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D689CD-3D77-4A6C-A4AF-3FE9E22D26E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1516380" y="2270760"/>
+          <a:ext cx="2651760" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you like to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> support - Buy me a coffe here:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://www.buymeacoffee.com/pro3d </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B62007A-FD2B-4F7A-92F8-47B0DD5F4710}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="914400" cy="906950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -835,6 +1089,75 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2651760" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{556CA2DE-563A-4278-AD31-D071EB004052}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200400" y="0"/>
+          <a:ext cx="2651760" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you like to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> support - Buy me a coffe here:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://www.buymeacoffee.com/pro3d </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1016,6 +1339,200 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1287780</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2651760" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73A11117-E615-4C72-9086-EB8CB0CF88D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1287780" y="213360"/>
+          <a:ext cx="2651760" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you like to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> support - Buy me a coffe here:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://www.buymeacoffee.com/pro3d </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>175430</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E7DCE86-35D8-4D1A-B225-5C3409657508}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="0"/>
+          <a:ext cx="914400" cy="906950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1234440</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2651760" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC3DD9BE-93ED-4542-935F-4F241F4A8A67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3726180" y="419100"/>
+          <a:ext cx="2651760" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If you like to</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> support - Buy me a coffe here:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://www.buymeacoffee.com/pro3d </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1340,7 +1857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
@@ -1349,105 +1866,112 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="37">
-        <f>'V-Slots and Wheels List'!F17</f>
+      <c r="B6" s="29">
+        <f>'V-Slots and Wheels List'!F18</f>
         <v>172.5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B7" s="29">
         <f>'Component Part List'!E28</f>
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B8" s="29">
         <f>'Fasteners List'!E33</f>
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="37"/>
-    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="36">
-        <f>SUM(B5:B8)</f>
+      <c r="B10" s="28">
+        <f>SUM(B6:B9)</f>
         <v>556.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A12" s="35" t="s">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A13" s="27" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1459,11 +1983,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{3FC4702C-93F0-44D6-B76F-6AAFF00BF8D8}"/>
-    <hyperlink ref="A5" location="'V-Slots and Wheels List'!A1" display="V-Slots and Wheels Standard Price:" xr:uid="{A29DA81D-7B91-4E4B-B65C-26042F66F5C3}"/>
-    <hyperlink ref="A6" location="'Component Part List'!A1" display="Components Example Price:" xr:uid="{9EB7D7DD-AF1E-400D-9685-4CB15F55C14B}"/>
-    <hyperlink ref="A7" location="'Fasteners List'!A1" display="Fastners Estimated Retail Price:" xr:uid="{542B85DB-19D3-4E26-AF3D-CED032A5654A}"/>
+    <hyperlink ref="A6" location="'V-Slots and Wheels List'!A1" display="V-Slots and Wheels Standard Price:" xr:uid="{A29DA81D-7B91-4E4B-B65C-26042F66F5C3}"/>
+    <hyperlink ref="A7" location="'Component Part List'!A1" display="Components Example Price:" xr:uid="{9EB7D7DD-AF1E-400D-9685-4CB15F55C14B}"/>
+    <hyperlink ref="A8" location="'Fasteners List'!A1" display="Fastners Estimated Retail Price:" xr:uid="{542B85DB-19D3-4E26-AF3D-CED032A5654A}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -1471,7 +1995,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
-  <dimension ref="A6:F17"/>
+  <dimension ref="A7:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1484,192 +2008,202 @@
     <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C7" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F7" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8" s="43">
-        <v>80</v>
-      </c>
-      <c r="F8" s="44">
-        <f>E8</f>
-        <v>80</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" s="37">
+        <v>80</v>
+      </c>
+      <c r="F9" s="38">
+        <f>E9</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9">
+      <c r="C10" s="36"/>
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11" s="26">
-        <v>5</v>
-      </c>
-      <c r="F11" s="26">
-        <f>E11*D11</f>
-        <v>20</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" s="18">
+        <v>5</v>
+      </c>
+      <c r="F12" s="18">
+        <f>E12*D12</f>
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C13" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E13" s="18">
         <v>5</v>
       </c>
-      <c r="F12" s="26">
-        <f>E12*D12</f>
+      <c r="F13" s="18">
+        <f>E13*D13</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15" s="26">
-        <v>3.5</v>
-      </c>
-      <c r="F15" s="7">
-        <f>E15*D15</f>
-        <v>31.5</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="F16" s="6">
+        <f>E16*D16</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C17" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D17" s="3">
         <v>12</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E17" s="18">
         <v>3</v>
       </c>
-      <c r="F16" s="26">
-        <f>E16*D16</f>
+      <c r="F17" s="18">
+        <f>E17*D17</f>
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="33">
-        <f>SUM(F8:F16)</f>
+      <c r="F18" s="25">
+        <f>SUM(F9:F17)</f>
         <v>172.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A21" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{03B994D7-7DDE-4DC5-8D5F-CB8F0AF1A502}"/>
-    <hyperlink ref="C16" r:id="rId2" xr:uid="{791129AB-97C1-4FA4-B7AE-F541BD16B51D}"/>
-    <hyperlink ref="C8:C9" r:id="rId3" display="Kit Link" xr:uid="{7D1A8CFE-30C0-4885-8FB7-D97F7761D013}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{D73E78DD-06D5-410D-ACC7-AF6B789FC2B1}"/>
-    <hyperlink ref="C12" r:id="rId5" xr:uid="{9E7C5336-3FF2-4EE3-AFBF-F1C41492D09C}"/>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{03B994D7-7DDE-4DC5-8D5F-CB8F0AF1A502}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{791129AB-97C1-4FA4-B7AE-F541BD16B51D}"/>
+    <hyperlink ref="C9:C10" r:id="rId3" display="Kit Link" xr:uid="{7D1A8CFE-30C0-4885-8FB7-D97F7761D013}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{D73E78DD-06D5-410D-ACC7-AF6B789FC2B1}"/>
+    <hyperlink ref="C13" r:id="rId5" xr:uid="{9E7C5336-3FF2-4EE3-AFBF-F1C41492D09C}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <drawing r:id="rId7"/>
 </worksheet>
@@ -1679,7 +2213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1691,39 +2227,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A1" s="6"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C7" t="s">
@@ -1732,7 +2268,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="20">
         <v>15</v>
       </c>
     </row>
@@ -1749,7 +2285,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="20">
         <v>10</v>
       </c>
     </row>
@@ -1757,7 +2293,7 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C9" t="s">
@@ -1766,7 +2302,7 @@
       <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="20">
         <v>4</v>
       </c>
     </row>
@@ -1774,7 +2310,7 @@
       <c r="A10" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C10" t="s">
@@ -1783,16 +2319,16 @@
       <c r="D10">
         <v>10</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="20">
         <v>15</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>99</v>
       </c>
       <c r="C11" t="s">
@@ -1801,7 +2337,7 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="20">
         <v>15</v>
       </c>
     </row>
@@ -1809,7 +2345,7 @@
       <c r="A12" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="22" t="s">
         <v>101</v>
       </c>
       <c r="C12" t="s">
@@ -1818,7 +2354,7 @@
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="20">
         <v>10</v>
       </c>
     </row>
@@ -1826,7 +2362,7 @@
       <c r="A13" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="22" t="s">
         <v>102</v>
       </c>
       <c r="C13" t="s">
@@ -1835,7 +2371,7 @@
       <c r="D13">
         <v>10</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="20">
         <v>10</v>
       </c>
     </row>
@@ -1843,7 +2379,7 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C14" t="s">
@@ -1852,7 +2388,7 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="20">
         <v>30</v>
       </c>
     </row>
@@ -1860,7 +2396,7 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1869,16 +2405,16 @@
       <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="20">
         <v>7</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C16" t="s">
@@ -1887,7 +2423,7 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="20">
         <v>25</v>
       </c>
     </row>
@@ -1895,7 +2431,7 @@
       <c r="A17" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C17" t="s">
@@ -1904,7 +2440,7 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="20">
         <v>4</v>
       </c>
     </row>
@@ -1912,7 +2448,7 @@
       <c r="A18" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C18" t="s">
@@ -1921,7 +2457,7 @@
       <c r="D18">
         <v>6</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="20">
         <v>3</v>
       </c>
     </row>
@@ -1929,7 +2465,7 @@
       <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1938,16 +2474,16 @@
       <c r="D19">
         <v>5</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="20">
         <v>40</v>
       </c>
-      <c r="F19" s="26"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C20" t="s">
@@ -1956,7 +2492,7 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="24">
         <v>10</v>
       </c>
       <c r="F20" t="s">
@@ -1967,7 +2503,7 @@
       <c r="A21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C21" t="s">
@@ -1976,7 +2512,7 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="24">
         <v>20</v>
       </c>
       <c r="F21" t="s">
@@ -1996,7 +2532,7 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="24">
         <v>20</v>
       </c>
       <c r="F22" t="s">
@@ -2007,7 +2543,7 @@
       <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C23" t="s">
@@ -2016,7 +2552,7 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="20">
         <v>20</v>
       </c>
     </row>
@@ -2033,7 +2569,7 @@
       <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="20">
         <v>10</v>
       </c>
     </row>
@@ -2050,7 +2586,7 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="20">
         <v>10</v>
       </c>
     </row>
@@ -2058,16 +2594,16 @@
       <c r="A26" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="10" t="s">
         <v>97</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="20">
         <v>20</v>
       </c>
     </row>
@@ -2075,7 +2611,7 @@
       <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C27" t="s">
@@ -2084,15 +2620,15 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="20">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="21">
         <f>SUM(E7:E27)</f>
         <v>308</v>
       </c>
@@ -2103,7 +2639,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2148,490 +2684,1294 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="9" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="B6" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="13">
         <v>10</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="42">
         <v>0.1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="40">
         <f>D8*C8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>10</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="42">
         <v>0.1</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="40">
         <f t="shared" ref="E9:E32" si="0">D9*C9</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="13">
         <v>20</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="42">
         <v>0.1</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="12">
         <v>10</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="42">
         <v>0.1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="13">
         <v>10</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="42">
         <v>0.1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="12">
         <v>20</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="42">
         <v>0.1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="13">
         <v>10</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="42">
         <v>0.1</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="12">
         <v>10</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="42">
         <v>0.1</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="13">
         <v>10</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="42">
         <v>0.1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <v>10</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="42">
         <v>0.1</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="13">
         <v>75</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="42">
         <v>0.1</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="40">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="12">
         <v>20</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="42">
         <v>0.1</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="13">
         <v>40</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="42">
         <v>0.1</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="40">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="12">
         <v>50</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="42">
         <v>0.1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="40">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="13">
         <v>25</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="42">
         <v>0.1</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="40">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="12">
         <v>75</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="42">
         <v>0.1</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="40">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="13">
         <v>150</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="42">
         <v>0.1</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="40">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="12">
         <v>100</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="42">
         <v>0.1</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="40">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="13">
         <v>10</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="42">
         <v>0.1</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="12">
         <v>20</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="42">
         <v>0.1</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="13">
         <v>10</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="42">
         <v>0.1</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="12">
         <v>20</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="42">
         <v>0.1</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="40">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="13">
         <v>10</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="42">
         <v>0.1</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="12">
         <v>10</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="42">
         <v>0.1</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="13">
         <v>25</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="42">
         <v>0.1</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="40">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="23">
         <f>SUM(E8:E32)</f>
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B772BFAF-98E7-48E2-B803-10D3054F2AAB}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="10">
+        <v>10</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="40">
+        <v>10</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="10">
+        <v>20</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="40">
+        <v>10</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="10">
+        <v>10</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="40">
+        <v>20</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="10">
+        <v>10</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="40">
+        <v>10</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="10">
+        <v>10</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="40">
+        <v>10</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="10">
+        <v>75</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="40">
+        <v>20</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="10">
+        <v>40</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="40">
+        <v>50</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="10">
+        <v>25</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="40">
+        <v>75</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="10">
+        <v>150</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="40">
+        <v>100</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="10">
+        <v>10</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="40">
+        <v>20</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="10">
+        <v>10</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="40"/>
+      <c r="C41" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="40">
+        <v>20</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="10">
+        <v>10</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="40">
+        <v>10</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="10">
+        <v>25</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="40">
+        <v>6</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F47" s="41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{84743980-7531-4764-B6BC-E90222E0915C}"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed controller board link to MKS Gen L
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{743FDE47-DC1B-48D3-9544-DCB70625E548}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{DD668C84-5A8D-413E-8BFA-84E8370B79EB}"/>
   <bookViews>
-    <workbookView xWindow="23400" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24336" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -253,9 +253,6 @@
     <t>Controller</t>
   </si>
   <si>
-    <t>MKS Gen 1.4</t>
-  </si>
-  <si>
     <t>Ramps Controller</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>V-King - Component Parts to Buy</t>
+  </si>
+  <si>
+    <t>MKS Gen L V1.0</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1871,7 +1871,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="29">
         <f>'V-Slots and Wheels List'!F18</f>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="29">
         <f>'Component Part List'!E28</f>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="29">
         <f>'Fasteners List'!E33</f>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="28">
         <f>SUM(B6:B9)</f>
@@ -1967,12 +1967,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A13" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2016,16 +2016,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,7 +2044,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9">
         <v>12</v>
@@ -2086,7 +2086,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -2107,7 +2107,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2134,10 +2134,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16">
         <v>9</v>
@@ -2155,10 +2155,10 @@
         <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="3">
         <v>12</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18" s="25">
         <f>SUM(F9:F17)</f>
@@ -2182,12 +2182,12 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2213,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,12 +2229,12 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2248,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="16"/>
     </row>
@@ -2297,7 +2297,7 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -2326,10 +2326,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2360,13 +2360,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
         <v>101</v>
-      </c>
-      <c r="C13" t="s">
-        <v>102</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2397,10 +2397,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2415,10 +2415,10 @@
         <v>62</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2432,10 +2432,10 @@
         <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>85</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2484,10 +2484,10 @@
         <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2496,7 +2496,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2504,10 +2504,10 @@
         <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2516,7 +2516,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2527,7 +2527,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2536,7 +2536,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2544,10 +2544,10 @@
         <v>72</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" t="s">
         <v>73</v>
-      </c>
-      <c r="C23" t="s">
-        <v>74</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2561,10 +2561,10 @@
         <v>72</v>
       </c>
       <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -2578,10 +2578,10 @@
         <v>72</v>
       </c>
       <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2598,7 +2598,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2612,10 +2612,10 @@
         <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
         <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E28" s="21">
         <f>SUM(E7:E27)</f>
@@ -2635,12 +2635,12 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2685,17 +2685,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="B6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2706,13 +2706,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3167,7 +3167,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" s="23">
         <f>SUM(E8:E32)</f>
@@ -3199,20 +3199,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3220,13 +3220,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>29</v>
@@ -3255,7 +3255,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3272,7 +3272,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3280,7 +3280,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -3292,18 +3292,18 @@
         <v>5</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
         <v>133</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3312,7 +3312,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3328,10 +3328,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -3340,7 +3340,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="3">
         <v>12</v>
@@ -3358,12 +3358,12 @@
         <v>5</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3373,7 +3373,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -3382,55 +3382,55 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -3443,7 +3443,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>36</v>
@@ -3455,7 +3455,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,7 +3463,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>57</v>
@@ -3475,7 +3475,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3483,7 +3483,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>56</v>
@@ -3495,7 +3495,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3503,7 +3503,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>30</v>
@@ -3515,7 +3515,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3533,7 +3533,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3541,7 +3541,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>30</v>
@@ -3553,7 +3553,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3561,7 +3561,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>59</v>
@@ -3573,7 +3573,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3591,7 +3591,7 @@
         <v>47</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3609,7 +3609,7 @@
         <v>47</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3627,7 +3627,7 @@
         <v>47</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3635,7 +3635,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>52</v>
@@ -3647,7 +3647,7 @@
         <v>47</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,7 +3665,7 @@
         <v>47</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3673,7 +3673,7 @@
         <v>39</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>53</v>
@@ -3685,7 +3685,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3693,7 +3693,7 @@
         <v>48</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" s="34" t="s">
         <v>49</v>
@@ -3705,7 +3705,7 @@
         <v>47</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3723,7 +3723,7 @@
         <v>47</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3741,7 +3741,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3749,7 +3749,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="34" t="s">
         <v>54</v>
@@ -3761,7 +3761,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3769,7 +3769,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>30</v>
@@ -3781,7 +3781,7 @@
         <v>47</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3799,7 +3799,7 @@
         <v>47</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3817,7 +3817,7 @@
         <v>47</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -3835,7 +3835,7 @@
         <v>47</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3853,7 +3853,7 @@
         <v>47</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3871,7 +3871,7 @@
         <v>47</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3889,7 +3889,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3907,7 +3907,7 @@
         <v>47</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3915,24 +3915,24 @@
         <v>50</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="34" t="s">
         <v>160</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>161</v>
       </c>
       <c r="D45" s="34">
         <v>6</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="1"/>
@@ -3942,27 +3942,27 @@
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding modular X carrier non probe
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{DD668C84-5A8D-413E-8BFA-84E8370B79EB}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{C9B13430-B4C8-464C-B62D-954BAEF0DE59}"/>
   <bookViews>
-    <workbookView xWindow="24336" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Fasteners List" sheetId="4" r:id="rId4"/>
     <sheet name="Bundle Order List" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="170">
   <si>
     <t>Part Name</t>
   </si>
@@ -394,9 +394,6 @@
     <t>Estimated Component Retail Price</t>
   </si>
   <si>
-    <t>Hotend</t>
-  </si>
-  <si>
     <t>Filament Extruder</t>
   </si>
   <si>
@@ -539,6 +536,12 @@
   </si>
   <si>
     <t>MKS Gen L V1.0</t>
+  </si>
+  <si>
+    <t>e3d Type Hotend</t>
+  </si>
+  <si>
+    <t>Titan Type Extruder</t>
   </si>
 </sst>
 </file>
@@ -1860,13 +1863,13 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
@@ -2003,7 +2006,7 @@
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2025,7 +2028,7 @@
         <v>93</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2211,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,7 +2232,7 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2484,10 +2487,10 @@
         <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2496,7 +2499,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2504,10 +2507,10 @@
         <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2516,7 +2519,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2527,7 +2530,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2536,7 +2539,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2544,7 +2547,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
@@ -2641,6 +2644,11 @@
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2662,10 +2670,11 @@
     <hyperlink ref="B12" r:id="rId15" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
     <hyperlink ref="B13" r:id="rId16" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
     <hyperlink ref="B15" r:id="rId17" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
+    <hyperlink ref="C36" r:id="rId18" xr:uid="{5027B5BA-4B7A-5345-A44A-1946DE4724CD}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2678,7 +2687,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3199,20 +3208,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3220,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>1</v>
@@ -3255,7 +3264,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3272,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3280,7 +3289,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -3292,18 +3301,18 @@
         <v>5</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
         <v>132</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3312,7 +3321,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3328,10 +3337,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -3340,7 +3349,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3349,7 +3358,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="3">
         <v>12</v>
@@ -3358,12 +3367,12 @@
         <v>5</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3373,7 +3382,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -3382,55 +3391,55 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -3443,7 +3452,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>36</v>
@@ -3455,7 +3464,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3463,7 +3472,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>57</v>
@@ -3475,7 +3484,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3483,7 +3492,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>56</v>
@@ -3495,7 +3504,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3503,7 +3512,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>30</v>
@@ -3515,7 +3524,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3533,7 +3542,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3541,7 +3550,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>30</v>
@@ -3553,7 +3562,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3561,7 +3570,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>59</v>
@@ -3573,7 +3582,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3591,7 +3600,7 @@
         <v>47</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3609,7 +3618,7 @@
         <v>47</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3627,7 +3636,7 @@
         <v>47</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3635,7 +3644,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>52</v>
@@ -3647,7 +3656,7 @@
         <v>47</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3665,7 +3674,7 @@
         <v>47</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3673,7 +3682,7 @@
         <v>39</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>53</v>
@@ -3685,7 +3694,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3693,7 +3702,7 @@
         <v>48</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" s="34" t="s">
         <v>49</v>
@@ -3705,7 +3714,7 @@
         <v>47</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3723,7 +3732,7 @@
         <v>47</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3741,7 +3750,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3749,7 +3758,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C36" s="34" t="s">
         <v>54</v>
@@ -3761,7 +3770,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3769,7 +3778,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>30</v>
@@ -3781,7 +3790,7 @@
         <v>47</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3799,7 +3808,7 @@
         <v>47</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3817,7 +3826,7 @@
         <v>47</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -3835,7 +3844,7 @@
         <v>47</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3853,7 +3862,7 @@
         <v>47</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3871,7 +3880,7 @@
         <v>47</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3889,7 +3898,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3907,7 +3916,7 @@
         <v>47</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3915,24 +3924,24 @@
         <v>50</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>160</v>
       </c>
       <c r="D45" s="34">
         <v>6</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="1"/>
@@ -3942,19 +3951,19 @@
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Changed link to bearings - Important
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{C9B13430-B4C8-464C-B62D-954BAEF0DE59}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{63074AD4-5A5D-496A-B66A-92BDF82626B8}"/>
   <bookViews>
     <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="170">
   <si>
     <t>Part Name</t>
   </si>
@@ -2216,9 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2647,9 +2645,7 @@
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="C36" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2670,11 +2666,10 @@
     <hyperlink ref="B12" r:id="rId15" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
     <hyperlink ref="B13" r:id="rId16" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
     <hyperlink ref="B15" r:id="rId17" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
-    <hyperlink ref="C36" r:id="rId18" xr:uid="{5027B5BA-4B7A-5345-A44A-1946DE4724CD}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId19"/>
-  <drawing r:id="rId20"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
deleted link to V-Slots
Finding new supplier
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{9E6A5CC3-4B24-4354-8ADB-C58105CFF206}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5E19315E-3191-41C4-9514-99068A246830}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="167">
   <si>
     <t>Part Name</t>
   </si>
@@ -307,16 +307,7 @@
     <t>350*400 Silicone Heatpad</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Link to shop</t>
-  </si>
-  <si>
     <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Kit Link</t>
   </si>
   <si>
     <t xml:space="preserve">240W 24V PSU </t>
@@ -1862,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -1874,7 +1865,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="37" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1888,7 +1879,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1902,7 +1893,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1930,7 +1921,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B6" s="29">
         <f>'V-Slots and Wheels List'!F18</f>
@@ -1939,7 +1930,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B7" s="29">
         <f>'Component Part List'!E28</f>
@@ -1948,7 +1939,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B8" s="29">
         <f>'Fasteners List'!E33</f>
@@ -1961,7 +1952,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B10" s="28">
         <f>SUM(B6:B9)</f>
@@ -1970,7 +1961,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
@@ -2000,7 +1991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
   <dimension ref="A7:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2018,17 +2011,15 @@
       <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>92</v>
-      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2046,9 +2037,7 @@
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>94</v>
-      </c>
+      <c r="C9" s="40"/>
       <c r="D9">
         <v>12</v>
       </c>
@@ -2088,9 +2077,7 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>91</v>
-      </c>
+      <c r="C12" s="17"/>
       <c r="D12">
         <v>4</v>
       </c>
@@ -2109,9 +2096,7 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>91</v>
-      </c>
+      <c r="C13" s="14"/>
       <c r="D13">
         <v>1</v>
       </c>
@@ -2137,11 +2122,9 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>91</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16">
         <v>9</v>
       </c>
@@ -2158,11 +2141,9 @@
         <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>91</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="3">
         <v>12</v>
       </c>
@@ -2176,7 +2157,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F18" s="25">
         <f>SUM(F9:F17)</f>
@@ -2199,16 +2180,9 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" xr:uid="{03B994D7-7DDE-4DC5-8D5F-CB8F0AF1A502}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{791129AB-97C1-4FA4-B7AE-F541BD16B51D}"/>
-    <hyperlink ref="C9:C10" r:id="rId3" display="Kit Link" xr:uid="{7D1A8CFE-30C0-4885-8FB7-D97F7761D013}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{D73E78DD-06D5-410D-ACC7-AF6B789FC2B1}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{9E7C5336-3FF2-4EE3-AFBF-F1C41492D09C}"/>
-  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-  <drawing r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2216,7 +2190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2232,7 +2206,7 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2311,10 +2285,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -2329,10 +2303,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
@@ -2346,13 +2320,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2363,13 +2337,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2400,10 +2374,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2487,10 +2461,10 @@
         <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2499,7 +2473,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2507,10 +2481,10 @@
         <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2519,7 +2493,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2530,7 +2504,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2539,7 +2513,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2547,7 +2521,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
@@ -2601,7 +2575,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2629,7 +2603,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E28" s="21">
         <f>SUM(E7:E27)</f>
@@ -2715,10 +2689,10 @@
         <v>87</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3173,7 +3147,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E33" s="23">
         <f>SUM(E8:E32)</f>
@@ -3205,20 +3179,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3226,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>1</v>
@@ -3261,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,7 +3252,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3286,7 +3260,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -3298,18 +3272,18 @@
         <v>5</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3318,7 +3292,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3334,10 +3308,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -3346,7 +3320,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3355,7 +3329,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" s="3">
         <v>12</v>
@@ -3364,12 +3338,12 @@
         <v>5</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3379,7 +3353,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -3388,55 +3362,55 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -3449,7 +3423,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>36</v>
@@ -3461,7 +3435,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3469,7 +3443,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>57</v>
@@ -3481,7 +3455,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3489,7 +3463,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>56</v>
@@ -3501,7 +3475,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,7 +3483,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>30</v>
@@ -3521,7 +3495,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3539,7 +3513,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3547,7 +3521,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>30</v>
@@ -3559,7 +3533,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3567,7 +3541,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>59</v>
@@ -3579,7 +3553,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3597,7 +3571,7 @@
         <v>47</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3615,7 +3589,7 @@
         <v>47</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3633,7 +3607,7 @@
         <v>47</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3641,7 +3615,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>52</v>
@@ -3653,7 +3627,7 @@
         <v>47</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3671,7 +3645,7 @@
         <v>47</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3679,7 +3653,7 @@
         <v>39</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>53</v>
@@ -3691,7 +3665,7 @@
         <v>47</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3699,7 +3673,7 @@
         <v>48</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C33" s="34" t="s">
         <v>49</v>
@@ -3711,7 +3685,7 @@
         <v>47</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3729,7 +3703,7 @@
         <v>47</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3747,7 +3721,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3755,7 +3729,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C36" s="34" t="s">
         <v>54</v>
@@ -3767,7 +3741,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3775,7 +3749,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>30</v>
@@ -3787,7 +3761,7 @@
         <v>47</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3805,7 +3779,7 @@
         <v>47</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3823,7 +3797,7 @@
         <v>47</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -3841,7 +3815,7 @@
         <v>47</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3859,7 +3833,7 @@
         <v>47</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3877,7 +3851,7 @@
         <v>47</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3895,7 +3869,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3913,7 +3887,7 @@
         <v>47</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3921,24 +3895,24 @@
         <v>50</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D45" s="34">
         <v>6</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="1"/>
@@ -3948,19 +3922,19 @@
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Updated V-Slot part list
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{8BA4C632-0229-43C4-85C3-2C2D4E862F72}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{C1498313-2324-4423-B4B8-550B61F67D4D}"/>
   <bookViews>
     <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
   <si>
     <t>Part Name</t>
   </si>
@@ -346,15 +346,9 @@
     <t>Corner Joint Brackets</t>
   </si>
   <si>
-    <t>Ratrig Retail Shop Price</t>
-  </si>
-  <si>
     <t>V-Slot Big Wheels - Z wheels</t>
   </si>
   <si>
-    <t>V-Slot Big Wheels - XY wheels</t>
-  </si>
-  <si>
     <t>Estimated fastener price in total:</t>
   </si>
   <si>
@@ -536,14 +530,19 @@
   </si>
   <si>
     <t>OpenBuilds</t>
+  </si>
+  <si>
+    <t>for V-Slots</t>
+  </si>
+  <si>
+    <t>Estimated Kit Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="[$EUR]\ #,##0.00"/>
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="[$EUR]\ #,##0.0"/>
     <numFmt numFmtId="166" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -705,7 +704,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -745,6 +743,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -755,13 +762,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1860,112 +1861,112 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="A2" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="28">
-        <f>'V-Slots and Wheels List'!F18</f>
-        <v>172.5</v>
+        <v>113</v>
+      </c>
+      <c r="B6" s="27">
+        <f>'V-Slots and Wheels List'!F17</f>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="28">
+        <v>108</v>
+      </c>
+      <c r="B7" s="27">
         <f>'Component Part List'!E28</f>
         <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="28">
+        <v>109</v>
+      </c>
+      <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="28"/>
+      <c r="B9" s="27"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="27">
+      <c r="A10" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>556.5</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1989,7 +1990,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
-  <dimension ref="A7:F21"/>
+  <dimension ref="A5:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2002,22 +2003,30 @@
     <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>166</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>121</v>
+      <c r="F7" s="15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2028,172 +2037,130 @@
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9" s="40">
-        <v>80</v>
-      </c>
-      <c r="F9" s="41">
-        <f>E9</f>
-        <v>80</v>
-      </c>
-    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="39"/>
+        <v>32</v>
+      </c>
+      <c r="C10" s="41"/>
       <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="16">
+        <v>5</v>
+      </c>
+      <c r="F10" s="16">
+        <f>E10*D10</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>5</v>
+      </c>
+      <c r="F11" s="16">
+        <f>E11*D11</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" s="36">
+        <v>3</v>
+      </c>
+      <c r="F12" s="16">
+        <f>E12*D12</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="3">
+        <v>21</v>
+      </c>
+      <c r="E15" s="16">
+        <v>3</v>
+      </c>
+      <c r="F15" s="16">
+        <f>E15*D15</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12" s="17">
-        <v>5</v>
-      </c>
-      <c r="F12" s="17">
-        <f>E12*D12</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="17">
-        <v>5</v>
-      </c>
-      <c r="F13" s="17">
-        <f>E13*D13</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16" s="17">
-        <v>3.5</v>
-      </c>
-      <c r="F16" s="6">
-        <f>E16*D16</f>
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="3">
-        <v>12</v>
-      </c>
-      <c r="E17" s="17">
-        <v>3</v>
-      </c>
-      <c r="F17" s="17">
-        <f>E17*D17</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="24">
-        <f>SUM(F9:F17)</f>
-        <v>172.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="F17" s="23">
+        <f>SUM(F10:F15)</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A21" s="8" t="s">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C17"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C9:C10" r:id="rId1" display="OpenBuilds" xr:uid="{9DE15799-91A0-4A8E-97E0-C7E44B6622BF}"/>
-    <hyperlink ref="C12:C13" r:id="rId2" display="OpenBuilds" xr:uid="{B47E854E-F919-4096-AEE8-C911C7ADBD0B}"/>
-    <hyperlink ref="C16:C17" r:id="rId3" display="OpenBuilds" xr:uid="{582B9A1C-4FD3-4CE1-9B1B-FA5E47AECF79}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{582B9A1C-4FD3-4CE1-9B1B-FA5E47AECF79}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2216,8 +2183,8 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
-      <c r="B1" s="9" t="s">
-        <v>163</v>
+      <c r="B1" s="8" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2226,22 +2193,22 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2256,7 +2223,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>15</v>
       </c>
     </row>
@@ -2273,7 +2240,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>10</v>
       </c>
     </row>
@@ -2290,7 +2257,7 @@
       <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2307,10 +2274,10 @@
       <c r="D10">
         <v>10</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <v>15</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2325,7 +2292,7 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="18">
         <v>15</v>
       </c>
     </row>
@@ -2333,7 +2300,7 @@
       <c r="A12" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>96</v>
       </c>
       <c r="C12" t="s">
@@ -2342,7 +2309,7 @@
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <v>10</v>
       </c>
     </row>
@@ -2350,7 +2317,7 @@
       <c r="A13" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
       <c r="C13" t="s">
@@ -2359,7 +2326,7 @@
       <c r="D13">
         <v>10</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <v>10</v>
       </c>
     </row>
@@ -2376,7 +2343,7 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <v>30</v>
       </c>
     </row>
@@ -2384,7 +2351,7 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2393,10 +2360,10 @@
       <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <v>7</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2411,7 +2378,7 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2428,7 +2395,7 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="18">
         <v>4</v>
       </c>
     </row>
@@ -2445,7 +2412,7 @@
       <c r="D18">
         <v>6</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <v>3</v>
       </c>
     </row>
@@ -2453,7 +2420,7 @@
       <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2462,29 +2429,29 @@
       <c r="D19">
         <v>5</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2492,19 +2459,19 @@
         <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2515,16 +2482,16 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2532,7 +2499,7 @@
         <v>72</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>73</v>
@@ -2540,7 +2507,7 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>20</v>
       </c>
     </row>
@@ -2557,7 +2524,7 @@
       <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="18">
         <v>10</v>
       </c>
     </row>
@@ -2574,7 +2541,7 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="18">
         <v>10</v>
       </c>
     </row>
@@ -2582,16 +2549,16 @@
       <c r="A26" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="18">
         <v>20</v>
       </c>
     </row>
@@ -2608,15 +2575,15 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="18">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="20">
+      <c r="A28" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="19">
         <f>SUM(E7:E27)</f>
         <v>308</v>
       </c>
@@ -2627,7 +2594,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2675,7 +2642,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2685,482 +2652,482 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>10</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>0.1</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <f>D8*C8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>10</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <v>0.1</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <f t="shared" ref="E9:E32" si="0">D9*C9</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>20</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <v>0.1</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>10</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <v>0.1</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>10</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <v>0.1</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>20</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="34">
         <v>0.1</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>10</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="34">
         <v>0.1</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>10</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="34">
         <v>0.1</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>10</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="34">
         <v>0.1</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>10</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="34">
         <v>0.1</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>75</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <v>0.1</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="32">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>20</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="34">
         <v>0.1</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <v>40</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <v>0.1</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>50</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <v>0.1</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <v>25</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="34">
         <v>0.1</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>75</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="34">
         <v>0.1</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="32">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <v>150</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="34">
         <v>0.1</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>100</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="34">
         <v>0.1</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="12">
         <v>10</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="34">
         <v>0.1</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="11">
         <v>20</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="34">
         <v>0.1</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="12">
         <v>10</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="34">
         <v>0.1</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="11">
         <v>20</v>
       </c>
-      <c r="D29" s="35">
+      <c r="D29" s="34">
         <v>0.1</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="12">
         <v>10</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="34">
         <v>0.1</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>10</v>
       </c>
-      <c r="D31" s="35">
+      <c r="D31" s="34">
         <v>0.1</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="12">
         <v>25</v>
       </c>
-      <c r="D32" s="35">
+      <c r="D32" s="34">
         <v>0.1</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="32">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="22">
+      <c r="A33" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
         <v>76</v>
       </c>
@@ -3189,40 +3156,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
-        <v>122</v>
+      <c r="B1" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -3245,8 +3212,8 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>126</v>
+      <c r="F8" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3262,8 +3229,8 @@
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>126</v>
+      <c r="F9" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3271,7 +3238,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -3282,19 +3249,19 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>126</v>
+      <c r="F10" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3302,8 +3269,8 @@
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="32" t="s">
-        <v>126</v>
+      <c r="F11" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3319,10 +3286,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D13">
         <v>9</v>
@@ -3330,8 +3297,8 @@
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>126</v>
+      <c r="F13" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3340,7 +3307,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D14" s="3">
         <v>12</v>
@@ -3348,13 +3315,13 @@
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>126</v>
+      <c r="F14" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3364,7 +3331,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -3373,55 +3340,55 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>126</v>
+        <v>134</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>126</v>
+        <v>134</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>126</v>
+        <v>134</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -3430,529 +3397,529 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="9">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="32">
+        <v>10</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="C22" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="9">
+        <v>20</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="32">
         <v>10</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="33">
+      <c r="F23" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="9">
         <v>10</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="33" t="s">
+      <c r="F24" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="C25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="32">
         <v>20</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="33" t="s">
+      <c r="F25" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C26" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="9">
+        <v>10</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="32">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D28" s="9">
         <v>10</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33" t="s">
+      <c r="F28" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D29" s="32">
         <v>10</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="33" t="s">
+      <c r="F29" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C30" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="9">
+        <v>75</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="32">
+        <v>20</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="9">
+        <v>40</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="32">
+        <v>50</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="9">
+        <v>25</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="32">
+        <v>75</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="9">
+        <v>150</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D37" s="32">
+        <v>100</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="9">
+        <v>10</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="32">
         <v>20</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="10">
+      <c r="F39" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="9">
         <v>10</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="33">
+      <c r="F40" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="32">
+        <v>20</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="9">
         <v>10</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="F42" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="32">
         <v>10</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="33">
-        <v>10</v>
-      </c>
-      <c r="E29" s="10" t="s">
+      <c r="F43" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="9">
+        <v>25</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="10">
-        <v>75</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="33">
-        <v>20</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="10">
-        <v>40</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="33">
+      <c r="F44" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="10">
-        <v>25</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="33">
-        <v>75</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="33" t="s">
+      <c r="B45" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="10">
-        <v>150</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="33" t="s">
+      <c r="C45" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="C37" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="33">
-        <v>100</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="10">
-        <v>10</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="33">
-        <v>20</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="10">
-        <v>10</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="33">
-        <v>20</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="10">
-        <v>10</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="33">
-        <v>10</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="10">
-        <v>25</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F44" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="33" t="s">
+      <c r="D45" s="32">
+        <v>6</v>
+      </c>
+      <c r="E45" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C45" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="33">
-        <v>6</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>126</v>
+      <c r="F45" s="31" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>161</v>
+        <v>134</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remobed bundle pdf until supplier in place
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{C1498313-2324-4423-B4B8-550B61F67D4D}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5F8E363C-CA5E-4E13-8816-234F250CD11F}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="145">
   <si>
     <t>Part Name</t>
   </si>
@@ -136,9 +136,6 @@
     <t>480mm V Slot</t>
   </si>
   <si>
-    <t>Xtreme Solid V Wheel Kit</t>
-  </si>
-  <si>
     <t>Solid V Wheel Kit</t>
   </si>
   <si>
@@ -394,108 +391,42 @@
     <t>Bulk Price</t>
   </si>
   <si>
-    <t>V-King Bundle List - Send this list to info@ratrig.com to order</t>
-  </si>
-  <si>
     <t>Estamated price for the bundle - 250 EUR - Ask for price confirmation</t>
   </si>
   <si>
-    <t>Mailto:</t>
-  </si>
-  <si>
-    <t>info@ratrig.com</t>
-  </si>
-  <si>
     <t>Standard</t>
   </si>
   <si>
-    <t>HW1113BC</t>
-  </si>
-  <si>
     <t xml:space="preserve">2028 L Bracket </t>
   </si>
   <si>
-    <t>HW1303BC</t>
-  </si>
-  <si>
     <t>28mm X 20mm corner bracket</t>
   </si>
   <si>
-    <t>HW1212WK</t>
-  </si>
-  <si>
-    <t>V-Slot Big Wheels - Extreme</t>
-  </si>
-  <si>
     <t>V-Slot Big Wheels - Standard</t>
   </si>
   <si>
     <t>Mechatronical components</t>
   </si>
   <si>
-    <t>HW1078EC</t>
-  </si>
-  <si>
     <t>Components</t>
   </si>
   <si>
     <t>Timing Belt GT2 6mm</t>
   </si>
   <si>
-    <t>HW1037GC</t>
-  </si>
-  <si>
     <t>Meter Timing belt for XYZ</t>
   </si>
   <si>
     <t>Timing Motor GT2 Pulley 20T</t>
   </si>
   <si>
-    <t>HW1035WC</t>
-  </si>
-  <si>
     <t>Motor Timing Pulleys</t>
   </si>
   <si>
     <t>Fastners and Bearings</t>
   </si>
   <si>
-    <t>HW1251NC</t>
-  </si>
-  <si>
-    <t>HW1508NC</t>
-  </si>
-  <si>
-    <t>HW1373NC</t>
-  </si>
-  <si>
-    <t>HW1505SC</t>
-  </si>
-  <si>
-    <t>HW1502SC</t>
-  </si>
-  <si>
-    <t>HW1561NC</t>
-  </si>
-  <si>
-    <t>HW1074NC</t>
-  </si>
-  <si>
-    <t>HW1039NC</t>
-  </si>
-  <si>
-    <t>HW1111NC</t>
-  </si>
-  <si>
-    <t>HW1315NC</t>
-  </si>
-  <si>
-    <t>HW1285SC</t>
-  </si>
-  <si>
-    <t>HW1209WC</t>
-  </si>
-  <si>
     <t>Ball Bearing - 625 ZZ</t>
   </si>
   <si>
@@ -505,9 +436,6 @@
     <t>Controller components</t>
   </si>
   <si>
-    <t>HW1351EC</t>
-  </si>
-  <si>
     <t>110/220VAC - 24V PSU 240W Min</t>
   </si>
   <si>
@@ -536,6 +464,9 @@
   </si>
   <si>
     <t>Estimated Kit Price</t>
+  </si>
+  <si>
+    <t>V-King Bundle List - Supplier to be decided</t>
   </si>
 </sst>
 </file>
@@ -543,8 +474,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$EUR]\ #,##0.0"/>
-    <numFmt numFmtId="166" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$EUR]\ #,##0.0"/>
+    <numFmt numFmtId="165" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -716,7 +647,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -725,11 +656,11 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -746,11 +677,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,9 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1865,46 +1796,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="A1" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
+      <c r="A3" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1922,7 +1853,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="27">
         <f>'V-Slots and Wheels List'!F17</f>
@@ -1931,7 +1862,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="27">
         <f>'Component Part List'!E28</f>
@@ -1940,7 +1871,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
@@ -1953,7 +1884,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
@@ -1962,12 +1893,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A13" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2005,10 +1936,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="35" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2023,10 +1954,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2044,7 +1975,7 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="38"/>
       <c r="D10">
         <v>16</v>
       </c>
@@ -2063,7 +1994,7 @@
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="38"/>
       <c r="D11">
         <v>1</v>
       </c>
@@ -2112,10 +2043,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="3">
         <v>21</v>
@@ -2137,7 +2068,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2146,12 +2077,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A20" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2168,9 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2184,12 +2113,12 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2203,22 +2132,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2229,13 +2158,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2246,13 +2175,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2263,13 +2192,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -2281,13 +2210,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2298,13 +2227,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2315,13 +2244,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
         <v>97</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2335,10 +2264,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>71</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2352,10 +2281,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2367,13 +2296,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2384,13 +2313,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2401,13 +2330,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
         <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2418,7 +2347,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>11</v>
@@ -2436,13 +2365,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2451,18 +2380,18 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2471,18 +2400,18 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2491,18 +2420,18 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" t="s">
-        <v>73</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2513,13 +2442,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -2530,13 +2459,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2547,13 +2476,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2564,13 +2493,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2581,7 +2510,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" s="19">
         <f>SUM(E7:E27)</f>
@@ -2590,12 +2519,12 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A31" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
@@ -2643,34 +2572,34 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="B6" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2678,7 +2607,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="12">
         <v>10</v>
@@ -2696,7 +2625,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="11">
         <v>10</v>
@@ -2714,7 +2643,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="12">
         <v>20</v>
@@ -2729,7 +2658,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>30</v>
@@ -2783,10 +2712,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="C14" s="12">
         <v>10</v>
@@ -2804,7 +2733,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="11">
         <v>10</v>
@@ -2855,10 +2784,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="12">
         <v>75</v>
@@ -2876,7 +2805,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="11">
         <v>20</v>
@@ -2891,10 +2820,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="12">
         <v>40</v>
@@ -2909,10 +2838,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="C21" s="11">
         <v>50</v>
@@ -2927,10 +2856,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="C22" s="12">
         <v>25</v>
@@ -2966,7 +2895,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="12">
         <v>150</v>
@@ -2999,7 +2928,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>30</v>
@@ -3017,10 +2946,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="C27" s="11">
         <v>20</v>
@@ -3089,10 +3018,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="11">
         <v>10</v>
@@ -3110,7 +3039,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="12">
         <v>25</v>
@@ -3125,7 +3054,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
@@ -3141,7 +3070,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B772BFAF-98E7-48E2-B803-10D3054F2AAB}">
-  <dimension ref="A1:F48"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3157,34 +3089,29 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>29</v>
@@ -3213,7 +3140,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,16 +3157,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>125</v>
-      </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3250,18 +3174,15 @@
         <v>5</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3270,7 +3191,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3285,43 +3206,31 @@
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>129</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
+        <v>123</v>
+      </c>
+      <c r="D13" s="3">
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="3">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>124</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3330,9 +3239,7 @@
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3340,596 +3247,578 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>136</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>139</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="9">
-        <v>10</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>124</v>
-      </c>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>143</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B21" s="32"/>
       <c r="C21" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="32">
+        <v>35</v>
+      </c>
+      <c r="D21" s="9">
         <v>10</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>144</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B22" s="32"/>
       <c r="C22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="9">
-        <v>20</v>
+      <c r="D22" s="32">
+        <v>10</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="32">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="9">
+        <v>20</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B24" s="32"/>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="32">
         <v>10</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="C25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="32">
-        <v>20</v>
+      <c r="D25" s="9">
+        <v>10</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="9">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="32">
+        <v>20</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="32">
+        <v>58</v>
+      </c>
+      <c r="D27" s="9">
         <v>10</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="32" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="9">
+        <v>54</v>
+      </c>
+      <c r="D28" s="32">
         <v>10</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" s="32"/>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="9">
         <v>10</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="9">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="32">
+        <v>10</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="32" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="32">
-        <v>20</v>
+        <v>51</v>
+      </c>
+      <c r="D31" s="9">
+        <v>75</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>149</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B32" s="32"/>
       <c r="C32" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="9">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D32" s="32">
+        <v>20</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>150</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B33" s="32"/>
       <c r="C33" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="32">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="D33" s="9">
+        <v>40</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B34" s="32"/>
       <c r="C34" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="9">
-        <v>25</v>
+        <v>48</v>
+      </c>
+      <c r="D34" s="32">
+        <v>50</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="32">
-        <v>75</v>
+        <v>40</v>
+      </c>
+      <c r="D35" s="9">
+        <v>25</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>151</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B36" s="32"/>
       <c r="C36" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="9">
-        <v>150</v>
+        <v>8</v>
+      </c>
+      <c r="D36" s="32">
+        <v>75</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="32">
-        <v>100</v>
+        <v>9</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="9">
+        <v>150</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="32" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B38" s="32"/>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="9">
-        <v>10</v>
+      <c r="D38" s="32">
+        <v>100</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="32"/>
       <c r="C39" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="32">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D39" s="9">
+        <v>10</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B40" s="32"/>
       <c r="C40" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="9">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="D40" s="32">
+        <v>20</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B41" s="32"/>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="32">
-        <v>20</v>
+      <c r="D41" s="9">
+        <v>10</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B42" s="32"/>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="9">
-        <v>10</v>
+      <c r="D42" s="32">
+        <v>20</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="32" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B43" s="32"/>
       <c r="C43" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="32">
+        <v>30</v>
+      </c>
+      <c r="D43" s="9">
         <v>10</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B44" s="32"/>
       <c r="C44" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="32">
+        <v>10</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="9">
-        <v>25</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="F44" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>153</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B45" s="32"/>
       <c r="C45" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="D45" s="32">
+        <v>45</v>
+      </c>
+      <c r="D45" s="9">
+        <v>25</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="32">
         <v>6</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F45" s="31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="E46" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D47">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49">
         <v>1</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" s="33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A48" t="s">
+      <c r="E49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{84743980-7531-4764-B6BC-E90222E0915C}"/>
-  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added 3d touch link
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5F8E363C-CA5E-4E13-8816-234F250CD11F}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{32BE98A4-9256-4B94-9616-9F3A33390586}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -220,9 +220,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>BL Touch Probe</t>
-  </si>
-  <si>
     <t>Optical Sensor</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
     <t>Filament Extruder</t>
   </si>
   <si>
-    <t>Autobed Leveling Probe</t>
-  </si>
-  <si>
     <t>Add Price</t>
   </si>
   <si>
@@ -467,6 +461,12 @@
   </si>
   <si>
     <t>V-King Bundle List - Supplier to be decided</t>
+  </si>
+  <si>
+    <t>3D Touch Probe</t>
+  </si>
+  <si>
+    <t>Original Probe here</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1797,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="27">
         <f>'V-Slots and Wheels List'!F17</f>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="27">
         <f>'Component Part List'!E28</f>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
@@ -1893,12 +1893,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A13" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
   <dimension ref="A5:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1936,10 +1936,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1954,10 +1954,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2046,7 +2046,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" s="3">
         <v>21</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2077,12 +2077,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2113,12 +2113,12 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2132,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -2161,10 +2161,10 @@
         <v>59</v>
       </c>
       <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2181,7 +2181,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2192,13 +2192,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -2210,13 +2210,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -2244,13 +2244,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
         <v>96</v>
-      </c>
-      <c r="C13" t="s">
-        <v>97</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2264,10 +2264,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2281,10 +2281,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2299,10 +2299,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2316,10 +2316,10 @@
         <v>61</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2333,10 +2333,10 @@
         <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2368,10 +2368,10 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2380,7 +2380,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2388,10 +2388,10 @@
         <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2400,18 +2400,18 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>115</v>
+      <c r="B22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2420,18 +2420,18 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
         <v>73</v>
-      </c>
-      <c r="C24" t="s">
-        <v>74</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -2459,13 +2459,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
         <v>75</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2476,13 +2476,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2496,10 +2496,10 @@
         <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="19">
         <f>SUM(E7:E27)</f>
@@ -2519,12 +2519,12 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A31" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
@@ -2549,10 +2549,12 @@
     <hyperlink ref="B12" r:id="rId15" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
     <hyperlink ref="B13" r:id="rId16" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
     <hyperlink ref="B15" r:id="rId17" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
+    <hyperlink ref="B22" r:id="rId18" display="BL Touch Probe" xr:uid="{4921FFD9-8616-4796-AF0F-67C77EA5A27C}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{D8FBE80D-6647-42BD-AA31-6FB3B8A2D48A}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId20"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -2572,17 +2574,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="B6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2593,13 +2595,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3054,7 +3056,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
@@ -3089,12 +3091,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3105,13 +3107,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>29</v>
@@ -3140,7 +3142,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3157,7 +3159,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3174,15 +3176,15 @@
         <v>5</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3191,7 +3193,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -3208,7 +3210,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3217,7 +3219,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3230,7 +3232,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3247,46 +3249,46 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3298,7 +3300,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3321,7 +3323,7 @@
         <v>46</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3339,7 +3341,7 @@
         <v>46</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3357,7 +3359,7 @@
         <v>46</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3375,7 +3377,7 @@
         <v>46</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3393,7 +3395,7 @@
         <v>46</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,7 +3413,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3429,7 +3431,7 @@
         <v>46</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3447,7 +3449,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3465,7 +3467,7 @@
         <v>46</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3483,7 +3485,7 @@
         <v>46</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3501,7 +3503,7 @@
         <v>46</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3519,7 +3521,7 @@
         <v>46</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3537,7 +3539,7 @@
         <v>46</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3555,7 +3557,7 @@
         <v>46</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3573,7 +3575,7 @@
         <v>46</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3591,7 +3593,7 @@
         <v>46</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3609,7 +3611,7 @@
         <v>46</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3627,7 +3629,7 @@
         <v>46</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3645,7 +3647,7 @@
         <v>46</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -3663,7 +3665,7 @@
         <v>46</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3681,7 +3683,7 @@
         <v>46</v>
       </c>
       <c r="F41" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3699,7 +3701,7 @@
         <v>46</v>
       </c>
       <c r="F42" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -3717,7 +3719,7 @@
         <v>46</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3735,7 +3737,7 @@
         <v>46</v>
       </c>
       <c r="F44" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3753,7 +3755,7 @@
         <v>46</v>
       </c>
       <c r="F45" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -3762,16 +3764,16 @@
       </c>
       <c r="B46" s="32"/>
       <c r="C46" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D46" s="32">
         <v>6</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F46" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -3784,7 +3786,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
@@ -3795,24 +3797,24 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F49" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added link to clone extruder
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/V-King/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{32BE98A4-9256-4B94-9616-9F3A33390586}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{F12500F0-ACA1-4C57-AF52-D1D4BD01FC50}"/>
   <bookViews>
     <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,9 +448,6 @@
     <t>e3d Type Hotend</t>
   </si>
   <si>
-    <t>Titan Type Extruder</t>
-  </si>
-  <si>
     <t>OpenBuilds</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>Original Probe here</t>
+  </si>
+  <si>
+    <t>Titan Original Here</t>
   </si>
 </sst>
 </file>
@@ -1936,10 +1936,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
         <v>139</v>
-      </c>
-      <c r="D5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2099,7 +2099,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2390,8 +2392,8 @@
       <c r="B21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C21" t="s">
-        <v>138</v>
+      <c r="C21" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2408,10 +2410,10 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2540,7 +2542,7 @@
     <hyperlink ref="B14" r:id="rId6" xr:uid="{94C4C13B-0BBB-4F7B-A730-B3205BF6E8ED}"/>
     <hyperlink ref="B23" r:id="rId7" xr:uid="{36DCFF59-08CA-412B-82D6-7AAD9283F4CA}"/>
     <hyperlink ref="B20" r:id="rId8" display="E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
-    <hyperlink ref="B21" r:id="rId9" display="Titan Extruder" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
+    <hyperlink ref="B21" r:id="rId9" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
     <hyperlink ref="B27" r:id="rId10" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
     <hyperlink ref="B17" r:id="rId11" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
     <hyperlink ref="B9" r:id="rId12" xr:uid="{2A7E1508-6E65-4E26-BF99-CF81B8D345E1}"/>
@@ -2551,10 +2553,11 @@
     <hyperlink ref="B15" r:id="rId17" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
     <hyperlink ref="B22" r:id="rId18" display="BL Touch Probe" xr:uid="{4921FFD9-8616-4796-AF0F-67C77EA5A27C}"/>
     <hyperlink ref="C22" r:id="rId19" xr:uid="{D8FBE80D-6647-42BD-AA31-6FB3B8A2D48A}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{55B76075-89E5-4B66-9E0E-72A33EE17BD5}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId20"/>
-  <drawing r:id="rId21"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -3091,7 +3094,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
reorgonizing files for simpler access
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{75628440-3626-43B7-9F57-39ECFCA90972}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D497BC22-05B6-44D9-9998-84D932CA1681}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="145">
   <si>
     <t>Part Name</t>
   </si>
@@ -382,9 +382,6 @@
     <t>Estamated price for the bundle - 250 EUR - Ask for price confirmation</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t xml:space="preserve">2028 L Bracket </t>
   </si>
   <si>
@@ -425,9 +422,6 @@
   </si>
   <si>
     <t>110/220VAC - 24V PSU 240W Min</t>
-  </si>
-  <si>
-    <t>Option</t>
   </si>
   <si>
     <t>Part Number</t>
@@ -483,7 +477,7 @@
     <numFmt numFmtId="164" formatCode="[$EUR]\ #,##0.0"/>
     <numFmt numFmtId="165" formatCode="_([$EUR]\ * #,##0_);_([$EUR]\ * \(#,##0\);_([$EUR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,15 +544,8 @@
       <name val="Aharoni"/>
       <charset val="177"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,17 +555,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,12 +605,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -676,9 +651,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -702,9 +675,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1398,10 +1370,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1234440</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2651760" cy="436786"/>
     <xdr:sp macro="" textlink="">
@@ -1418,7 +1390,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3726180" y="419100"/>
+          <a:off x="1638300" y="411480"/>
           <a:ext cx="2651760" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1802,46 +1774,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1941,11 +1913,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="35" t="s">
-        <v>136</v>
+      <c r="C5" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1981,7 +1953,7 @@
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="36"/>
       <c r="D10">
         <v>16</v>
       </c>
@@ -2000,7 +1972,7 @@
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="36"/>
       <c r="D11">
         <v>1</v>
       </c>
@@ -2019,11 +1991,11 @@
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="33"/>
       <c r="D12">
         <v>8</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="34">
         <v>3</v>
       </c>
       <c r="F12" s="16">
@@ -2034,9 +2006,9 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="C13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -2074,7 +2046,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2105,9 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2121,7 +2091,7 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2172,7 +2142,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2310,7 +2280,7 @@
         <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2379,7 +2349,7 @@
         <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2399,7 +2369,7 @@
         <v>111</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2416,10 +2386,10 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2436,7 +2406,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2521,10 +2491,10 @@
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2643,10 +2613,10 @@
       <c r="C8" s="12">
         <v>10</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="32">
         <v>0.1</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f>D8*C8</f>
         <v>1</v>
       </c>
@@ -2661,10 +2631,10 @@
       <c r="C9" s="11">
         <v>10</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <v>0.1</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <f t="shared" ref="E9:E32" si="0">D9*C9</f>
         <v>1</v>
       </c>
@@ -2679,10 +2649,10 @@
       <c r="C10" s="12">
         <v>20</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="32">
         <v>0.1</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2697,10 +2667,10 @@
       <c r="C11" s="11">
         <v>10</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="32">
         <v>0.1</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2715,10 +2685,10 @@
       <c r="C12" s="12">
         <v>10</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="32">
         <v>0.1</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2733,10 +2703,10 @@
       <c r="C13" s="11">
         <v>20</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="32">
         <v>0.1</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2751,10 +2721,10 @@
       <c r="C14" s="12">
         <v>10</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="32">
         <v>0.1</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2769,10 +2739,10 @@
       <c r="C15" s="11">
         <v>10</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="32">
         <v>0.1</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2787,10 +2757,10 @@
       <c r="C16" s="12">
         <v>10</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="32">
         <v>0.1</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2805,10 +2775,10 @@
       <c r="C17" s="11">
         <v>10</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>0.1</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2823,10 +2793,10 @@
       <c r="C18" s="12">
         <v>75</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="32">
         <v>0.1</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -2841,10 +2811,10 @@
       <c r="C19" s="11">
         <v>20</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="32">
         <v>0.1</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2859,10 +2829,10 @@
       <c r="C20" s="12">
         <v>40</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="32">
         <v>0.1</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2877,10 +2847,10 @@
       <c r="C21" s="11">
         <v>50</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>0.1</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2895,10 +2865,10 @@
       <c r="C22" s="12">
         <v>25</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="32">
         <v>0.1</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -2913,10 +2883,10 @@
       <c r="C23" s="11">
         <v>75</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="32">
         <v>0.1</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="31">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -2931,10 +2901,10 @@
       <c r="C24" s="12">
         <v>150</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="32">
         <v>0.1</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2949,10 +2919,10 @@
       <c r="C25" s="11">
         <v>100</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="32">
         <v>0.1</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2967,10 +2937,10 @@
       <c r="C26" s="12">
         <v>10</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="32">
         <v>0.1</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2985,10 +2955,10 @@
       <c r="C27" s="11">
         <v>20</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="32">
         <v>0.1</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3003,10 +2973,10 @@
       <c r="C28" s="12">
         <v>10</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="32">
         <v>0.1</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3021,10 +2991,10 @@
       <c r="C29" s="11">
         <v>20</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="32">
         <v>0.1</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="31">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3039,10 +3009,10 @@
       <c r="C30" s="12">
         <v>10</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="32">
         <v>0.1</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3057,10 +3027,10 @@
       <c r="C31" s="11">
         <v>10</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="32">
         <v>0.1</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3075,10 +3045,10 @@
       <c r="C32" s="12">
         <v>25</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="32">
         <v>0.1</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -3104,9 +3074,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3115,28 +3085,27 @@
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
@@ -3147,9 +3116,8 @@
       <c r="E6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -3157,7 +3125,7 @@
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3170,11 +3138,8 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -3187,11 +3152,8 @@
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3204,16 +3166,13 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="31" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3221,11 +3180,8 @@
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -3233,13 +3189,13 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3247,26 +3203,22 @@
       <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="31"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -3278,58 +3230,48 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="31"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3337,12 +3279,12 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="9">
@@ -3351,34 +3293,28 @@
       <c r="E21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <v>10</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="32" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="31" t="s">
         <v>55</v>
       </c>
       <c r="D23" s="9">
@@ -3387,34 +3323,28 @@
       <c r="E23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>10</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="9">
@@ -3423,34 +3353,28 @@
       <c r="E25" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>20</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D27" s="9">
@@ -3459,34 +3383,28 @@
       <c r="E27" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>10</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="9">
@@ -3495,34 +3413,28 @@
       <c r="E29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="32" t="s">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="31">
         <v>10</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="9">
@@ -3531,34 +3443,28 @@
       <c r="E31" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32" t="s">
+      <c r="B32" s="31"/>
+      <c r="C32" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="31">
         <v>20</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32" t="s">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="9">
@@ -3567,34 +3473,28 @@
       <c r="E33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32" t="s">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="31">
         <v>50</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31" t="s">
         <v>40</v>
       </c>
       <c r="D35" s="9">
@@ -3603,34 +3503,28 @@
       <c r="E35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <v>75</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="32" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32" t="s">
+      <c r="B37" s="31"/>
+      <c r="C37" s="31" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="9">
@@ -3639,34 +3533,28 @@
       <c r="E37" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="32"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="31"/>
       <c r="C38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="31">
         <v>100</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="32" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32" t="s">
+      <c r="B39" s="31"/>
+      <c r="C39" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D39" s="9">
@@ -3675,34 +3563,28 @@
       <c r="E39" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="32" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32" t="s">
+      <c r="B40" s="31"/>
+      <c r="C40" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="31">
         <v>20</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D41" s="9">
@@ -3711,34 +3593,28 @@
       <c r="E41" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D42" s="31">
         <v>20</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="32" t="s">
+      <c r="B43" s="31"/>
+      <c r="C43" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D43" s="9">
@@ -3747,34 +3623,28 @@
       <c r="E43" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="32" t="s">
+      <c r="B44" s="31"/>
+      <c r="C44" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="32">
+      <c r="D44" s="31">
         <v>10</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32" t="s">
+      <c r="B45" s="31"/>
+      <c r="C45" s="31" t="s">
         <v>45</v>
       </c>
       <c r="D45" s="9">
@@ -3783,62 +3653,52 @@
       <c r="E45" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32" t="s">
+      <c r="B46" s="31"/>
+      <c r="C46" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="31">
+        <v>6</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="32">
-        <v>6</v>
-      </c>
-      <c r="E46" s="9" t="s">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="F46" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="31"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F49" s="33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Updated links to pulleys
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D497BC22-05B6-44D9-9998-84D932CA1681}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{103468E1-D7A0-461B-B25C-79B0075F00EE}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="B7" s="27">
         <f>'Component Part List'!E29</f>
-        <v>320</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>568</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2077,7 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2182,7 +2182,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="18">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" s="6"/>
     </row>
@@ -2200,7 +2200,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="18">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2214,10 +2214,10 @@
         <v>89</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="E29" s="19">
         <f>SUM(E7:E28)</f>
-        <v>320</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3076,7 +3076,7 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
updated component links + added source file
Thumbscrew added to sf
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{103468E1-D7A0-461B-B25C-79B0075F00EE}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{C7DA080D-9228-45CF-AE66-9C2264187E8A}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -373,9 +373,6 @@
     <t>Add Price</t>
   </si>
   <si>
-    <t>J-Head/E3d Hotend</t>
-  </si>
-  <si>
     <t>Bulk Price</t>
   </si>
   <si>
@@ -433,9 +430,6 @@
     <t>MKS Gen L V1.0</t>
   </si>
   <si>
-    <t>e3d Type Hotend</t>
-  </si>
-  <si>
     <t>OpenBuilds</t>
   </si>
   <si>
@@ -467,6 +461,12 @@
   </si>
   <si>
     <t>5mm X 560mm Steel rod</t>
+  </si>
+  <si>
+    <t>J-Head/E3d Clone</t>
+  </si>
+  <si>
+    <t>e3d V6 Original Here</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1076,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -1763,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="B7" s="27">
         <f>'Component Part List'!E29</f>
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>553</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1914,10 +1914,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>87</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2046,7 +2046,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2077,7 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2091,7 +2091,7 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2142,7 +2142,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2280,7 +2280,7 @@
         <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2346,16 +2346,16 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" t="s">
-        <v>133</v>
+        <v>143</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" s="22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
         <v>112</v>
@@ -2369,7 +2369,7 @@
         <v>111</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2386,10 +2386,10 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2406,7 +2406,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2491,16 +2491,16 @@
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="18">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="E29" s="19">
         <f>SUM(E7:E28)</f>
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2534,7 +2534,7 @@
     <hyperlink ref="B11" r:id="rId5" xr:uid="{0BA4E21B-2D6F-419E-BB1C-022ED717A36F}"/>
     <hyperlink ref="B14" r:id="rId6" xr:uid="{94C4C13B-0BBB-4F7B-A730-B3205BF6E8ED}"/>
     <hyperlink ref="B23" r:id="rId7" xr:uid="{36DCFF59-08CA-412B-82D6-7AAD9283F4CA}"/>
-    <hyperlink ref="B20" r:id="rId8" display="E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
+    <hyperlink ref="B20" r:id="rId8" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
     <hyperlink ref="B21" r:id="rId9" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
     <hyperlink ref="B27" r:id="rId10" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
     <hyperlink ref="B17" r:id="rId11" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
@@ -2550,10 +2550,11 @@
     <hyperlink ref="B28" r:id="rId21" xr:uid="{20CA74F6-9B49-4A6D-8DB6-16AFDE7D4641}"/>
     <hyperlink ref="B24" r:id="rId22" xr:uid="{B94573F1-B78C-47F1-B3ED-C228D2514D12}"/>
     <hyperlink ref="B25" r:id="rId23" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
+    <hyperlink ref="C20" r:id="rId24" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
-  <drawing r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -3089,12 +3090,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3105,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
@@ -3169,10 +3170,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3195,7 +3196,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3213,7 +3214,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3230,37 +3231,37 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3271,7 +3272,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3660,13 +3661,13 @@
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="31">
         <v>6</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -3678,7 +3679,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
@@ -3689,13 +3690,13 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
changed rod lenght to 555
</commit_message>
<xml_diff>
--- a/BOM/V-King PRO 400 Part Order List.xlsx
+++ b/BOM/V-King PRO 400 Part Order List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{C7DA080D-9228-45CF-AE66-9C2264187E8A}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{FC616191-BDC2-4A19-95EA-3BDF8126B4A4}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Fasteners List" sheetId="4" r:id="rId4"/>
     <sheet name="Bundle Order List" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -460,13 +460,13 @@
     <t>Ask for 110 AC if needed</t>
   </si>
   <si>
-    <t>5mm X 560mm Steel rod</t>
-  </si>
-  <si>
     <t>J-Head/E3d Clone</t>
   </si>
   <si>
     <t>e3d V6 Original Here</t>
+  </si>
+  <si>
+    <t>5mm X 555 mm Steel rod</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -2077,7 +2077,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2142,7 +2144,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2346,10 +2348,10 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="D20">
         <v>1</v>

</xml_diff>